<commit_message>
Update PARTNER1 description. closes #12
</commit_message>
<xml_diff>
--- a/tables/ERAP Action recommendation reference.xlsx
+++ b/tables/ERAP Action recommendation reference.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc.edwards\Documents\PROJECTS\Canada_wide_ecoregion_assessments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc.edwards\Documents\Github\erap_code\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97ED8FB-C2D2-4650-8848-9B46F75A33C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE4303B-A043-4FB2-8D41-7796758F5897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{21822EA7-ACAB-4588-9BDD-7167B7C23A8A}"/>
   </bookViews>
@@ -146,9 +146,6 @@
     <t>10.3 Alliance &amp; Partnership Development</t>
   </si>
   <si>
-    <t>NCC owns fee-simple land and a Land Sharing plan is required</t>
-  </si>
-  <si>
     <t>Area of NCC fee-simple land</t>
   </si>
   <si>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>PARTNER1</t>
+  </si>
+  <si>
+    <t>NCC owns fee-simple land. Consider appropriate land sharing strategies.</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -749,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -761,7 +761,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -769,7 +769,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
@@ -789,7 +789,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>9</v>
@@ -809,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>13</v>
@@ -829,7 +829,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>17</v>
@@ -849,7 +849,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>21</v>
@@ -869,7 +869,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>26</v>
@@ -881,7 +881,7 @@
         <v>28</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -889,13 +889,13 @@
         <v>29</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>31</v>
@@ -909,16 +909,16 @@
         <v>29</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>34</v>
@@ -929,19 +929,19 @@
         <v>35</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>36</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>37</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>28</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add better names for actions. closes #15
</commit_message>
<xml_diff>
--- a/tables/ERAP Action recommendation reference.xlsx
+++ b/tables/ERAP Action recommendation reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc.edwards\Documents\Github\erap_code\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE4303B-A043-4FB2-8D41-7796758F5897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26026762-EA67-4EC4-87A6-1C59040C43AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{21822EA7-ACAB-4588-9BDD-7167B7C23A8A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>Action CMP 2.0</t>
   </si>
@@ -183,6 +183,36 @@
   </si>
   <si>
     <t>NCC owns fee-simple land. Consider appropriate land sharing strategies.</t>
+  </si>
+  <si>
+    <t>Map viewer name</t>
+  </si>
+  <si>
+    <t>Area-based conservation - 30x30 goals</t>
+  </si>
+  <si>
+    <t>Ecosystem &amp; Natural Process (Re)Creation - opportunities</t>
+  </si>
+  <si>
+    <t>Ecosystem &amp; Natural Process (Re)Creation - 30x30 goals</t>
+  </si>
+  <si>
+    <t>Alliance &amp; Partnership Development - land sharing</t>
+  </si>
+  <si>
+    <t>Site / Area stewardship</t>
+  </si>
+  <si>
+    <t>Area-based conservation - endemic SAR</t>
+  </si>
+  <si>
+    <t>Area-based conservation - SAR</t>
+  </si>
+  <si>
+    <t>Area-based conservation - biodiversity urgency</t>
+  </si>
+  <si>
+    <t>Area-based conservation - biodiversity opportunities</t>
   </si>
 </sst>
 </file>
@@ -728,219 +758,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A66282-6C59-4618-A46B-15D995499505}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="104.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.7265625" customWidth="1"/>
-    <col min="4" max="4" width="61.1796875" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.7265625" customWidth="1"/>
+    <col min="2" max="2" width="66.1796875" customWidth="1"/>
+    <col min="3" max="3" width="50.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.7265625" customWidth="1"/>
+    <col min="5" max="5" width="61.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="C6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="C10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="D10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="E10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="F10" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="G10" s="17" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>